<commit_message>
Fill empty predicted prices
</commit_message>
<xml_diff>
--- a/Code/Data/DAX30/Efficient Portfolios with Prediction/Auto Recurrence/input 30/DAX30_efficient_portfolios_and_returns_with_prediction_annual.xlsx
+++ b/Code/Data/DAX30/Efficient Portfolios with Prediction/Auto Recurrence/input 30/DAX30_efficient_portfolios_and_returns_with_prediction_annual.xlsx
@@ -595,79 +595,79 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.1149941288671107</v>
+        <v>0.1150142238523799</v>
       </c>
       <c r="F2" t="n">
-        <v>0.07768077627931667</v>
+        <v>0.07444253671929686</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01352965653926533</v>
+        <v>0.04297320332665566</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01929625338712531</v>
+        <v>0.06618677344691688</v>
       </c>
       <c r="I2" t="n">
-        <v>0.07774511631771618</v>
+        <v>0.0637461350876069</v>
       </c>
       <c r="J2" t="n">
-        <v>0.02850878472628341</v>
+        <v>0.05031381695787946</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0280391914836548</v>
+        <v>0.01237727010568302</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08090159832413422</v>
+        <v>0.04385617353419044</v>
       </c>
       <c r="M2" t="n">
-        <v>9.616296144854669e-05</v>
+        <v>0.002825542626888368</v>
       </c>
       <c r="N2" t="n">
-        <v>0.004271135400916427</v>
+        <v>0.01508332367802973</v>
       </c>
       <c r="O2" t="n">
-        <v>0.08528566863909885</v>
+        <v>0.0727130859024976</v>
       </c>
       <c r="P2" t="n">
-        <v>0.05656014724444198</v>
+        <v>0.08046351491515639</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.08610522916108215</v>
+        <v>0.08038956857402742</v>
       </c>
       <c r="R2" t="n">
-        <v>0.05431941764142771</v>
+        <v>0.07292596336419167</v>
       </c>
       <c r="S2" t="n">
-        <v>0.004845319844063939</v>
+        <v>0.0428618797867517</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0192203621512863</v>
+        <v>0.002148174181858787</v>
       </c>
       <c r="U2" t="n">
-        <v>0.01662099030077757</v>
+        <v>0.04868719933942547</v>
       </c>
       <c r="V2" t="n">
-        <v>0.01468733850279676</v>
+        <v>0.01204303254533616</v>
       </c>
       <c r="W2" t="n">
-        <v>0.07599259603656679</v>
+        <v>0.07736357033831984</v>
       </c>
       <c r="X2" t="n">
-        <v>0.03479081134954212</v>
+        <v>0.04368910570213181</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.0625717976258766</v>
+        <v>0.03296108994200852</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.05151553655078565</v>
+        <v>0.03787537272190711</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.06092749949879375</v>
+        <v>0.02284702615724805</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.04648861003359905</v>
+        <v>0.001226641045992089</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.1799971775558545</v>
+        <v>0.1368066542523479</v>
       </c>
     </row>
     <row r="3">
@@ -690,79 +690,79 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.1251886914453234</v>
+        <v>0.1233629766334731</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02281463988523496</v>
+        <v>0.01653724262101531</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03130803569590394</v>
+        <v>0.0430955033845046</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03576594599056809</v>
+        <v>0.008717033393179549</v>
       </c>
       <c r="I3" t="n">
-        <v>0.07962214487978703</v>
+        <v>0.0979262414151959</v>
       </c>
       <c r="J3" t="n">
-        <v>0.008376964584818344</v>
+        <v>0.010004012400653</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0199009167349387</v>
+        <v>0.001138225865628304</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0328626527305164</v>
+        <v>0.01288754692428029</v>
       </c>
       <c r="M3" t="n">
-        <v>0.007981686836424579</v>
+        <v>0.004557047658630185</v>
       </c>
       <c r="N3" t="n">
-        <v>0.03826155748381971</v>
+        <v>0.06001568799645902</v>
       </c>
       <c r="O3" t="n">
-        <v>0.05159452616786394</v>
+        <v>0.02926630334073683</v>
       </c>
       <c r="P3" t="n">
-        <v>0.04640521911119531</v>
+        <v>0.001495460622486102</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.03125902708870628</v>
+        <v>0.05736090806723943</v>
       </c>
       <c r="R3" t="n">
-        <v>0.04226470467465208</v>
+        <v>0.0798952130062542</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0909658696486705</v>
+        <v>0.07826019239348818</v>
       </c>
       <c r="T3" t="n">
-        <v>0.0928507140684704</v>
+        <v>0.05756215846155461</v>
       </c>
       <c r="U3" t="n">
-        <v>0.05289101975389974</v>
+        <v>0.04885867363749846</v>
       </c>
       <c r="V3" t="n">
-        <v>0.02110712134001136</v>
+        <v>0.001368718108096502</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04696746549131559</v>
+        <v>0.04971179383559975</v>
       </c>
       <c r="X3" t="n">
-        <v>0.03474076439675419</v>
+        <v>0.09783120176150259</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.05990999770415121</v>
+        <v>0.08431188259248379</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.00493467213327218</v>
+        <v>0.02359175163055646</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.03901264717569822</v>
+        <v>0.05963274008709774</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1082017064233273</v>
+        <v>0.07597446079585912</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1597674881756737</v>
+        <v>0.151757487907815</v>
       </c>
     </row>
     <row r="4">
@@ -785,79 +785,79 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.1224788292446968</v>
+        <v>0.120132051740435</v>
       </c>
       <c r="F4" t="n">
-        <v>0.07224791294501784</v>
+        <v>0.07653344759693083</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05713540252297174</v>
+        <v>0.004235340914438088</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003171227501708565</v>
+        <v>0.009026601027684452</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0008612045304779663</v>
+        <v>0.04365040048061496</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1004610047049624</v>
+        <v>0.07160388155443599</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01483114219484387</v>
+        <v>0.002970274131913347</v>
       </c>
       <c r="L4" t="n">
-        <v>0.01399561733104451</v>
+        <v>0.008839556331585032</v>
       </c>
       <c r="M4" t="n">
-        <v>0.01187046945310738</v>
+        <v>0.04978122004694095</v>
       </c>
       <c r="N4" t="n">
-        <v>0.08269925435746196</v>
+        <v>0.006138092664991795</v>
       </c>
       <c r="O4" t="n">
-        <v>0.06117949998547032</v>
+        <v>0.04529174709583938</v>
       </c>
       <c r="P4" t="n">
-        <v>0.05499572089612181</v>
+        <v>0.0567050862451866</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.01442319434831212</v>
+        <v>0.06157422658164078</v>
       </c>
       <c r="R4" t="n">
-        <v>0.05105365629364712</v>
+        <v>0.06818775369159288</v>
       </c>
       <c r="S4" t="n">
-        <v>0.001114715415859589</v>
+        <v>0.0581243546320946</v>
       </c>
       <c r="T4" t="n">
-        <v>0.02673730019295316</v>
+        <v>0.0469411898802595</v>
       </c>
       <c r="U4" t="n">
-        <v>0.06563711502052529</v>
+        <v>0.07096220457344896</v>
       </c>
       <c r="V4" t="n">
-        <v>0.08734693089474632</v>
+        <v>0.05916507242013297</v>
       </c>
       <c r="W4" t="n">
-        <v>0.03325995642497026</v>
+        <v>0.07707556274728279</v>
       </c>
       <c r="X4" t="n">
-        <v>0.07625723101453057</v>
+        <v>0.08634416746788423</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.05067353655647455</v>
+        <v>0.03927807580792771</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.07487796794711694</v>
+        <v>0.05622437170627351</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.01555770559836179</v>
+        <v>0.0004939683571574705</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.02961223386931412</v>
+        <v>0.0008534040437430156</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.7190392063081569</v>
+        <v>-0.5894039106372533</v>
       </c>
     </row>
     <row r="5">
@@ -880,79 +880,79 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.1508827894676995</v>
+        <v>0.1742925923512308</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08700230795780318</v>
+        <v>0.06009099459452791</v>
       </c>
       <c r="G5" t="n">
-        <v>0.003940801120399366</v>
+        <v>0.05501450391872826</v>
       </c>
       <c r="H5" t="n">
-        <v>0.04916941416202388</v>
+        <v>0.09384045143284524</v>
       </c>
       <c r="I5" t="n">
-        <v>0.08643100299156051</v>
+        <v>0.1000825904311536</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01702747117176118</v>
+        <v>0.0783113243826295</v>
       </c>
       <c r="K5" t="n">
-        <v>0.02142175826306513</v>
+        <v>0.01266958662207113</v>
       </c>
       <c r="L5" t="n">
-        <v>0.07041176387177156</v>
+        <v>0.02837533434363052</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0005105603964159527</v>
+        <v>0.005773731538075956</v>
       </c>
       <c r="N5" t="n">
-        <v>0.02232125361727549</v>
+        <v>0.02501373973125455</v>
       </c>
       <c r="O5" t="n">
-        <v>0.05851077726850651</v>
+        <v>0.01932508242791479</v>
       </c>
       <c r="P5" t="n">
-        <v>0.007251436872644776</v>
+        <v>0.01848753392832615</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0782776986765957</v>
+        <v>0.08307764938736824</v>
       </c>
       <c r="R5" t="n">
-        <v>0.01909814339518379</v>
+        <v>0.102501733349014</v>
       </c>
       <c r="S5" t="n">
-        <v>0.08895960463795465</v>
+        <v>0.003143639436228302</v>
       </c>
       <c r="T5" t="n">
-        <v>0.030977332747384</v>
+        <v>0.0001270686836437951</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0474193590821887</v>
+        <v>0.003706264333909883</v>
       </c>
       <c r="V5" t="n">
-        <v>0.05325123310473399</v>
+        <v>0.04671426592205867</v>
       </c>
       <c r="W5" t="n">
-        <v>0.09479002706633531</v>
+        <v>0.004112062983270871</v>
       </c>
       <c r="X5" t="n">
-        <v>0.01450368805512883</v>
+        <v>0.007939557919739396</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.01502052251621529</v>
+        <v>0.05005087552756619</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.02877310873399083</v>
+        <v>0.01135355931545406</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.01970187031733396</v>
+        <v>0.05231301158480626</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.08522886397372725</v>
+        <v>0.1379754382057828</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.682226915903259</v>
+        <v>-0.664820011691355</v>
       </c>
     </row>
     <row r="6">
@@ -975,79 +975,79 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.2406395335780585</v>
+        <v>0.2336272105450075</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05981978457414004</v>
+        <v>0.09679329475100848</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04431910837816713</v>
+        <v>0.03818564262917924</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02932503773489725</v>
+        <v>0.008802321643678683</v>
       </c>
       <c r="I6" t="n">
-        <v>0.07527741870401045</v>
+        <v>0.01809881849156154</v>
       </c>
       <c r="J6" t="n">
-        <v>0.03563468922364565</v>
+        <v>0.0153941494114435</v>
       </c>
       <c r="K6" t="n">
-        <v>0.009023905771632753</v>
+        <v>0.02797397125974875</v>
       </c>
       <c r="L6" t="n">
-        <v>0.006231435201495474</v>
+        <v>0.0203387068190321</v>
       </c>
       <c r="M6" t="n">
-        <v>0.03925710632009063</v>
+        <v>0.001449595668143965</v>
       </c>
       <c r="N6" t="n">
-        <v>0.007381844766172407</v>
+        <v>0.006492889536629929</v>
       </c>
       <c r="O6" t="n">
-        <v>0.03424951978702</v>
+        <v>0.07880787174867705</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0819461144236166</v>
+        <v>0.01881969309516727</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.005080497381150694</v>
+        <v>0.05007092716513766</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06206340819309566</v>
+        <v>0.0926352027662927</v>
       </c>
       <c r="S6" t="n">
-        <v>0.06831345392886189</v>
+        <v>0.0402063266550575</v>
       </c>
       <c r="T6" t="n">
-        <v>0.03142782183884363</v>
+        <v>0.03586050488098916</v>
       </c>
       <c r="U6" t="n">
-        <v>0.04139936047719948</v>
+        <v>0.1146452508456209</v>
       </c>
       <c r="V6" t="n">
-        <v>0.01757499835464694</v>
+        <v>0.0003498632519966194</v>
       </c>
       <c r="W6" t="n">
-        <v>0.07785766810161819</v>
+        <v>0.08400483730434284</v>
       </c>
       <c r="X6" t="n">
-        <v>0.05011048028796076</v>
+        <v>0.03583588672555844</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.05019377879032248</v>
+        <v>0.1146897785093806</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.04570107960872739</v>
+        <v>0.0006740539271224125</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.04502368157430329</v>
+        <v>0.02282455341904851</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.0827878065783814</v>
+        <v>0.07704585949518207</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.2111215740668457</v>
+        <v>0.1949573316843213</v>
       </c>
     </row>
     <row r="7">
@@ -1070,79 +1070,79 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.3130116590425998</v>
+        <v>0.3617204077602578</v>
       </c>
       <c r="F7" t="n">
-        <v>0.06608322416985113</v>
+        <v>0.04203671834871904</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04167397894344392</v>
+        <v>0.02194056631680976</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01275842671922581</v>
+        <v>0.0180972555270071</v>
       </c>
       <c r="I7" t="n">
-        <v>0.04466570112495024</v>
+        <v>0.01615511104217845</v>
       </c>
       <c r="J7" t="n">
-        <v>0.029041730906065</v>
+        <v>0.04968211771451289</v>
       </c>
       <c r="K7" t="n">
-        <v>3.860773141441699e-05</v>
+        <v>0.02323692000791463</v>
       </c>
       <c r="L7" t="n">
-        <v>0.02844099570778913</v>
+        <v>0.06552593430273485</v>
       </c>
       <c r="M7" t="n">
-        <v>0.02626159545182269</v>
+        <v>0.02667646221414457</v>
       </c>
       <c r="N7" t="n">
-        <v>0.07922055477910663</v>
+        <v>0.07042911388113847</v>
       </c>
       <c r="O7" t="n">
-        <v>0.002850324947811503</v>
+        <v>0.007268835170931821</v>
       </c>
       <c r="P7" t="n">
-        <v>0.02034677214902862</v>
+        <v>0.04969366677948491</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.003118569473338004</v>
+        <v>0.01657251540173259</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0995892590217564</v>
+        <v>0.06621274856694059</v>
       </c>
       <c r="S7" t="n">
-        <v>0.008112580563557752</v>
+        <v>0.05655269695759698</v>
       </c>
       <c r="T7" t="n">
-        <v>0.02396187393339199</v>
+        <v>0.04318520569847886</v>
       </c>
       <c r="U7" t="n">
-        <v>0.01691023280482169</v>
+        <v>0.0203095100167856</v>
       </c>
       <c r="V7" t="n">
-        <v>0.08277934724123731</v>
+        <v>0.1191775631894225</v>
       </c>
       <c r="W7" t="n">
-        <v>0.07534945823708883</v>
+        <v>0.01481027957635738</v>
       </c>
       <c r="X7" t="n">
-        <v>0.09599534240923224</v>
+        <v>0.1233614649449139</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.03288571701668632</v>
+        <v>0.03327739329656801</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.09154376531823706</v>
+        <v>0.06268085653415305</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.02670919088005017</v>
+        <v>0.0046388761798509</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.09166275047009308</v>
+        <v>0.04847818833162307</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.3194810420341266</v>
+        <v>0.3609675607314082</v>
       </c>
     </row>
     <row r="8">
@@ -1165,79 +1165,79 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.2536464313467132</v>
+        <v>0.2483899539260424</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03019308767619642</v>
+        <v>0.03478872995162438</v>
       </c>
       <c r="G8" t="n">
-        <v>0.006657271323512195</v>
+        <v>0.009396467333953207</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01807567849744022</v>
+        <v>0.02268792452773166</v>
       </c>
       <c r="I8" t="n">
-        <v>0.08884939775740078</v>
+        <v>0.03921165422712306</v>
       </c>
       <c r="J8" t="n">
-        <v>0.009287283289539802</v>
+        <v>0.008053305397894943</v>
       </c>
       <c r="K8" t="n">
-        <v>0.011026600694816</v>
+        <v>0.009702846003907931</v>
       </c>
       <c r="L8" t="n">
-        <v>0.003295030116434728</v>
+        <v>0.09650439728120219</v>
       </c>
       <c r="M8" t="n">
-        <v>0.07039453123680711</v>
+        <v>0.005635601500755577</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0240406135449731</v>
+        <v>0.006372357669812124</v>
       </c>
       <c r="O8" t="n">
-        <v>0.04387297510124784</v>
+        <v>0.06266425993341887</v>
       </c>
       <c r="P8" t="n">
-        <v>0.03031985571142868</v>
+        <v>0.08316328049781158</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.01187975272812259</v>
+        <v>0.0133790858867544</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06869335224870468</v>
+        <v>0.09663492218950902</v>
       </c>
       <c r="S8" t="n">
-        <v>0.0609815112893498</v>
+        <v>0.03390378089893741</v>
       </c>
       <c r="T8" t="n">
-        <v>0.04050420450860929</v>
+        <v>0.05988465282517103</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0320668291056171</v>
+        <v>0.01097196325849797</v>
       </c>
       <c r="V8" t="n">
-        <v>0.00880605768424019</v>
+        <v>0.01097110554026566</v>
       </c>
       <c r="W8" t="n">
-        <v>0.08265146524123149</v>
+        <v>0.07774635467095201</v>
       </c>
       <c r="X8" t="n">
-        <v>0.06335107189525561</v>
+        <v>0.07819780897875098</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.06623782900870534</v>
+        <v>0.09590465902225745</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.08318450368559008</v>
+        <v>0.09192328237119238</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.07096529588209115</v>
+        <v>0.01094119350645608</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.07466580177268584</v>
+        <v>0.04136036652601979</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.09924851518327044</v>
+        <v>0.07354668053834672</v>
       </c>
     </row>
     <row r="9">
@@ -1260,79 +1260,79 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.2915106962300523</v>
+        <v>0.3073694280589266</v>
       </c>
       <c r="F9" t="n">
-        <v>0.007415960407110257</v>
+        <v>0.02167282983134594</v>
       </c>
       <c r="G9" t="n">
-        <v>0.007521375811314914</v>
+        <v>0.05273232737984427</v>
       </c>
       <c r="H9" t="n">
-        <v>0.07141258193715629</v>
+        <v>0.006016054490874227</v>
       </c>
       <c r="I9" t="n">
-        <v>0.03801795275708088</v>
+        <v>0.05211111994243486</v>
       </c>
       <c r="J9" t="n">
-        <v>0.09288389391124258</v>
+        <v>0.05278018283430096</v>
       </c>
       <c r="K9" t="n">
-        <v>0.036381138734181</v>
+        <v>0.08447054120748532</v>
       </c>
       <c r="L9" t="n">
-        <v>0.08032469943140239</v>
+        <v>0.004279477607703684</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0007540139335152493</v>
+        <v>0.01533991283515506</v>
       </c>
       <c r="N9" t="n">
-        <v>0.02531478737013839</v>
+        <v>0.09153956858266811</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01131012307388253</v>
+        <v>0.05751887169322978</v>
       </c>
       <c r="P9" t="n">
-        <v>0.01247684408856678</v>
+        <v>0.00865190757575832</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.02452509206662767</v>
+        <v>0.01639769709752753</v>
       </c>
       <c r="R9" t="n">
-        <v>0.09136958565000705</v>
+        <v>0.08032982440961194</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1074521088680529</v>
+        <v>0.06911337161977736</v>
       </c>
       <c r="T9" t="n">
-        <v>0.03855424790568964</v>
+        <v>0.01527000075252352</v>
       </c>
       <c r="U9" t="n">
-        <v>0.02533875081674275</v>
+        <v>0.04701293162493049</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1159590540227106</v>
+        <v>0.09389424220547317</v>
       </c>
       <c r="W9" t="n">
-        <v>0.001104446341767798</v>
+        <v>0.01406424960025444</v>
       </c>
       <c r="X9" t="n">
-        <v>0.01021169060755691</v>
+        <v>0.003009724166639598</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1023259233715002</v>
+        <v>0.00775394880522809</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.03865483401139018</v>
+        <v>0.09987209841650141</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.00110469328490628</v>
+        <v>0.01704547090579245</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.05958620159745684</v>
+        <v>0.08912364641493944</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.233087260037546</v>
+        <v>0.2199300457789388</v>
       </c>
     </row>
     <row r="10">
@@ -1355,79 +1355,79 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.1669564438498313</v>
+        <v>0.1648565903593187</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08340560435734894</v>
+        <v>0.004526706199917952</v>
       </c>
       <c r="G10" t="n">
-        <v>0.09056397280766984</v>
+        <v>0.04581691584739345</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0659046817633628</v>
+        <v>0.002148821570079614</v>
       </c>
       <c r="I10" t="n">
-        <v>0.03135580233335371</v>
+        <v>0.01825665149944337</v>
       </c>
       <c r="J10" t="n">
-        <v>0.008663629542139907</v>
+        <v>0.0173630917546054</v>
       </c>
       <c r="K10" t="n">
-        <v>0.006018290973168622</v>
+        <v>0.0328829328471265</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01738723851279114</v>
+        <v>0.001663032031798081</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0001565653621133572</v>
+        <v>0.02081213983812472</v>
       </c>
       <c r="N10" t="n">
-        <v>0.03815225883576989</v>
+        <v>0.00418754443277248</v>
       </c>
       <c r="O10" t="n">
-        <v>0.05291812242989466</v>
+        <v>0.09592612896688138</v>
       </c>
       <c r="P10" t="n">
-        <v>0.07064216401036132</v>
+        <v>0.07898446690368195</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.04612551800667124</v>
+        <v>0.09611830260827248</v>
       </c>
       <c r="R10" t="n">
-        <v>0.09373756513036771</v>
+        <v>0.06826491797153941</v>
       </c>
       <c r="S10" t="n">
-        <v>0.06544747537405188</v>
+        <v>0.07082867520800586</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0007056437821609299</v>
+        <v>0.04275868369916647</v>
       </c>
       <c r="U10" t="n">
-        <v>0.06165793167325419</v>
+        <v>0.05139453868841696</v>
       </c>
       <c r="V10" t="n">
-        <v>0.01519078107106419</v>
+        <v>0.004128208548849994</v>
       </c>
       <c r="W10" t="n">
-        <v>0.06742961430449466</v>
+        <v>0.0854052710533959</v>
       </c>
       <c r="X10" t="n">
-        <v>0.08342948410364205</v>
+        <v>0.03386220729017287</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.04878026425977416</v>
+        <v>0.06035750646784786</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.04032514595920642</v>
+        <v>0.1024499437740967</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.004249644171285423</v>
+        <v>0.05975553248597915</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.007752601236052594</v>
+        <v>0.002107780312431571</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.07981281016173351</v>
+        <v>-0.09915195987464515</v>
       </c>
     </row>
     <row r="11">
@@ -1450,79 +1450,79 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.202504128217007</v>
+        <v>0.2198199728118782</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04058971542698517</v>
+        <v>0.06057667171725107</v>
       </c>
       <c r="G11" t="n">
-        <v>0.05210755975675532</v>
+        <v>0.0616890958449725</v>
       </c>
       <c r="H11" t="n">
-        <v>0.04145131880261513</v>
+        <v>0.08746459942388909</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01705534518974556</v>
+        <v>0.02272345011508091</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1091988638663955</v>
+        <v>0.0868812125546007</v>
       </c>
       <c r="K11" t="n">
-        <v>0.06233257054317592</v>
+        <v>0.06268793842249992</v>
       </c>
       <c r="L11" t="n">
-        <v>0.03005896919086336</v>
+        <v>0.01106811849542906</v>
       </c>
       <c r="M11" t="n">
-        <v>0.006618274000646684</v>
+        <v>0.01066903748760649</v>
       </c>
       <c r="N11" t="n">
-        <v>0.02201958186164557</v>
+        <v>0.02354982312114582</v>
       </c>
       <c r="O11" t="n">
-        <v>0.01764123812051117</v>
+        <v>0.01063867412788821</v>
       </c>
       <c r="P11" t="n">
-        <v>0.02209894477831641</v>
+        <v>0.06237028559376807</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.009277660868988782</v>
+        <v>0.03586835207660826</v>
       </c>
       <c r="R11" t="n">
-        <v>0.1128999694101714</v>
+        <v>0.03004483553259492</v>
       </c>
       <c r="S11" t="n">
-        <v>0.05402920684253226</v>
+        <v>0.08420906234229697</v>
       </c>
       <c r="T11" t="n">
-        <v>0.006380091536483465</v>
+        <v>0.002616619329142483</v>
       </c>
       <c r="U11" t="n">
-        <v>0.06412265192992196</v>
+        <v>0.06085494512038699</v>
       </c>
       <c r="V11" t="n">
-        <v>0.08891193671963621</v>
+        <v>0.08640726196212352</v>
       </c>
       <c r="W11" t="n">
-        <v>0.08929002599322637</v>
+        <v>0.02644481970946832</v>
       </c>
       <c r="X11" t="n">
-        <v>0.002770359573019103</v>
+        <v>0.00741533941417597</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.03970137355833585</v>
+        <v>0.01101256653913153</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.07825241169787633</v>
+        <v>0.04450503112765974</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.02951078293254041</v>
+        <v>0.05387034931477686</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.00368114739961221</v>
+        <v>0.05643191062750252</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.07436785178986915</v>
+        <v>-0.1049376900259882</v>
       </c>
     </row>
     <row r="12">
@@ -1545,79 +1545,79 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.1701879776834769</v>
+        <v>0.1662278917984207</v>
       </c>
       <c r="F12" t="n">
-        <v>0.07757803192632914</v>
+        <v>0.03022804203971566</v>
       </c>
       <c r="G12" t="n">
-        <v>0.02229209394080669</v>
+        <v>0.009718132802490799</v>
       </c>
       <c r="H12" t="n">
-        <v>0.008271710198554152</v>
+        <v>0.05814468340465276</v>
       </c>
       <c r="I12" t="n">
-        <v>0.05136066197511781</v>
+        <v>0.09529679228129337</v>
       </c>
       <c r="J12" t="n">
-        <v>0.003415331929203636</v>
+        <v>0.004441892986162655</v>
       </c>
       <c r="K12" t="n">
-        <v>0.02092023512441566</v>
+        <v>0.009310036032667513</v>
       </c>
       <c r="L12" t="n">
-        <v>0.02329747567963324</v>
+        <v>0.06194555123589626</v>
       </c>
       <c r="M12" t="n">
-        <v>0.03638146712995545</v>
+        <v>0.05498835991255726</v>
       </c>
       <c r="N12" t="n">
-        <v>0.03342737461674286</v>
+        <v>0.006830930511521613</v>
       </c>
       <c r="O12" t="n">
-        <v>0.02379850512015739</v>
+        <v>0.05624239709074507</v>
       </c>
       <c r="P12" t="n">
-        <v>0.04730837734366433</v>
+        <v>0.09577617544417391</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.03242178003072022</v>
+        <v>0.02368025202379231</v>
       </c>
       <c r="R12" t="n">
-        <v>0.07685357971250702</v>
+        <v>0.09264500429627018</v>
       </c>
       <c r="S12" t="n">
-        <v>0.08029932800122266</v>
+        <v>0.03760638037644021</v>
       </c>
       <c r="T12" t="n">
-        <v>0.008098544356725702</v>
+        <v>0.01715361307817731</v>
       </c>
       <c r="U12" t="n">
-        <v>0.05460744986885204</v>
+        <v>0.0951753119110078</v>
       </c>
       <c r="V12" t="n">
-        <v>0.005709404200081609</v>
+        <v>0.01358977503536703</v>
       </c>
       <c r="W12" t="n">
-        <v>0.07496403714208999</v>
+        <v>0.1075546824956236</v>
       </c>
       <c r="X12" t="n">
-        <v>0.06472809431031069</v>
+        <v>0.0150280661047413</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.005744464625237171</v>
+        <v>0.0361289348277932</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.08426082090667439</v>
+        <v>0.03606067937342784</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.07956232363491475</v>
+        <v>0.04233266764153995</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.08469890822608338</v>
+        <v>0.0001216390939423658</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.2073654396371108</v>
+        <v>0.1762767618603444</v>
       </c>
     </row>
     <row r="13">
@@ -1640,79 +1640,79 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.1801017019379305</v>
+        <v>0.1887511184653686</v>
       </c>
       <c r="F13" t="n">
-        <v>0.09161109167752979</v>
+        <v>0.07838926126607165</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01953945916914734</v>
+        <v>0.01251716351868187</v>
       </c>
       <c r="H13" t="n">
-        <v>0.02305219902261398</v>
+        <v>0.02911527741143425</v>
       </c>
       <c r="I13" t="n">
-        <v>0.02680653953284781</v>
+        <v>0.03082820107224695</v>
       </c>
       <c r="J13" t="n">
-        <v>0.001179559350749035</v>
+        <v>0.04282230047663038</v>
       </c>
       <c r="K13" t="n">
-        <v>0.08338927474711681</v>
+        <v>0.06519405354163202</v>
       </c>
       <c r="L13" t="n">
-        <v>0.04591303423523726</v>
+        <v>0.1000473596938274</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0003605866269452446</v>
+        <v>0.006848062203186871</v>
       </c>
       <c r="N13" t="n">
-        <v>0.02374374937600385</v>
+        <v>0.03303942743478249</v>
       </c>
       <c r="O13" t="n">
-        <v>0.03984945096962836</v>
+        <v>0.03471956310996219</v>
       </c>
       <c r="P13" t="n">
-        <v>0.07467426270851658</v>
+        <v>0.04322389312285625</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.007394944695710517</v>
+        <v>0.01780109081443275</v>
       </c>
       <c r="R13" t="n">
-        <v>0.09617500160808064</v>
+        <v>0.001510140866021182</v>
       </c>
       <c r="S13" t="n">
-        <v>0.06229241919961167</v>
+        <v>0.118209036526398</v>
       </c>
       <c r="T13" t="n">
-        <v>0.03484183516336897</v>
+        <v>0.04896316293008013</v>
       </c>
       <c r="U13" t="n">
-        <v>0.02545407304257558</v>
+        <v>0.0155685417816336</v>
       </c>
       <c r="V13" t="n">
-        <v>0.01082212214678519</v>
+        <v>0.004032432536612051</v>
       </c>
       <c r="W13" t="n">
-        <v>0.09486830545629332</v>
+        <v>0.1202838744378106</v>
       </c>
       <c r="X13" t="n">
-        <v>0.007054176840540291</v>
+        <v>0.02391346466811389</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.03051039442750489</v>
+        <v>0.008397129435206869</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.09639803653836117</v>
+        <v>0.08628679931831765</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.01634973242389696</v>
+        <v>0.02868634160090008</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.08771975104093473</v>
+        <v>0.04960342223316092</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.2326007907021551</v>
+        <v>0.2465503712838998</v>
       </c>
     </row>
     <row r="14">
@@ -1735,79 +1735,79 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.1767208890821626</v>
+        <v>0.1739161088311904</v>
       </c>
       <c r="F14" t="n">
-        <v>0.09248301489030233</v>
+        <v>0.02180482714047145</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01679083786459509</v>
+        <v>0.01029419377911094</v>
       </c>
       <c r="H14" t="n">
-        <v>0.009881658317838575</v>
+        <v>0.06996199015702362</v>
       </c>
       <c r="I14" t="n">
-        <v>0.04324362179735398</v>
+        <v>0.04906222666473035</v>
       </c>
       <c r="J14" t="n">
-        <v>0.01298394741427273</v>
+        <v>0.0303226643297809</v>
       </c>
       <c r="K14" t="n">
-        <v>0.004726166210631748</v>
+        <v>0.001193494224876268</v>
       </c>
       <c r="L14" t="n">
-        <v>0.02278918258947144</v>
+        <v>0.02717741810431663</v>
       </c>
       <c r="M14" t="n">
-        <v>0.02471051159509799</v>
+        <v>0.07208450478215785</v>
       </c>
       <c r="N14" t="n">
-        <v>0.008143713812328122</v>
+        <v>0.001192212020795762</v>
       </c>
       <c r="O14" t="n">
-        <v>0.01192419878159906</v>
+        <v>0.06418025270619188</v>
       </c>
       <c r="P14" t="n">
-        <v>0.02492812726738287</v>
+        <v>0.08538637281554419</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.00648997325946989</v>
+        <v>0.05200123939349419</v>
       </c>
       <c r="R14" t="n">
-        <v>0.1058433023706088</v>
+        <v>0.08239702387093242</v>
       </c>
       <c r="S14" t="n">
-        <v>0.08451226195337844</v>
+        <v>0.03800906881953009</v>
       </c>
       <c r="T14" t="n">
-        <v>0.05983838820077498</v>
+        <v>0.001343262181902396</v>
       </c>
       <c r="U14" t="n">
-        <v>0.04462950997798665</v>
+        <v>0.08865843412219335</v>
       </c>
       <c r="V14" t="n">
-        <v>0.05581945810087487</v>
+        <v>0.02391360049731407</v>
       </c>
       <c r="W14" t="n">
-        <v>0.1358285946796585</v>
+        <v>0.0321790182281058</v>
       </c>
       <c r="X14" t="n">
-        <v>0.06373647710327755</v>
+        <v>0.07479955874441623</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.03907147735802788</v>
+        <v>0.0396618892947548</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.06973349210367416</v>
+        <v>0.062329000831241</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.05532743109370161</v>
+        <v>0.06525233233772383</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.006564653257692715</v>
+        <v>0.006795414953391942</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.18217975458178</v>
+        <v>0.1828727996501382</v>
       </c>
     </row>
     <row r="15">
@@ -1830,79 +1830,79 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.2066310879891792</v>
+        <v>0.192969391884182</v>
       </c>
       <c r="F15" t="n">
-        <v>0.07799985950728719</v>
+        <v>0.1167265706761278</v>
       </c>
       <c r="G15" t="n">
-        <v>0.05490545225097385</v>
+        <v>0.0633796743226234</v>
       </c>
       <c r="H15" t="n">
-        <v>0.02422397498542634</v>
+        <v>0.0404030831377739</v>
       </c>
       <c r="I15" t="n">
-        <v>0.08380261648262918</v>
+        <v>0.06529727309251643</v>
       </c>
       <c r="J15" t="n">
-        <v>0.04824306577865141</v>
+        <v>0.00201169702338823</v>
       </c>
       <c r="K15" t="n">
-        <v>0.07833401873478048</v>
+        <v>0.08485954888697697</v>
       </c>
       <c r="L15" t="n">
-        <v>0.04686451242529633</v>
+        <v>0.01057846092892294</v>
       </c>
       <c r="M15" t="n">
-        <v>0.02631691175811625</v>
+        <v>0.001795103244526417</v>
       </c>
       <c r="N15" t="n">
-        <v>0.01575480234901356</v>
+        <v>0.005843395688596741</v>
       </c>
       <c r="O15" t="n">
-        <v>0.06855241565702436</v>
+        <v>0.08923018071629123</v>
       </c>
       <c r="P15" t="n">
-        <v>0.006399103230410304</v>
+        <v>0.07513849207354172</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.002887818301000591</v>
+        <v>0.005552515841670918</v>
       </c>
       <c r="R15" t="n">
-        <v>0.0341008899214018</v>
+        <v>0.04875538072608356</v>
       </c>
       <c r="S15" t="n">
-        <v>0.05153692917253153</v>
+        <v>0.07385364129344696</v>
       </c>
       <c r="T15" t="n">
-        <v>0.01101102418262621</v>
+        <v>0.02370446135812235</v>
       </c>
       <c r="U15" t="n">
-        <v>0.01883338334803174</v>
+        <v>0.0901112104226614</v>
       </c>
       <c r="V15" t="n">
-        <v>0.0121350457227055</v>
+        <v>0.00224940565194952</v>
       </c>
       <c r="W15" t="n">
-        <v>0.07006660590989124</v>
+        <v>0.02362273953273273</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1031347001974605</v>
+        <v>0.04975693621978323</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.006340664744026603</v>
+        <v>0.05718272318285485</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.05695355249564618</v>
+        <v>0.007283076600027138</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.01156133866944595</v>
+        <v>0.008474982395815763</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.09004131417562278</v>
+        <v>0.05418944698356586</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.2413995453802562</v>
+        <v>0.2536714900321475</v>
       </c>
     </row>
     <row r="16">
@@ -1925,79 +1925,79 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.1359474022350762</v>
+        <v>0.1390617762455736</v>
       </c>
       <c r="F16" t="n">
-        <v>0.03033620386213119</v>
+        <v>0.07493372226137335</v>
       </c>
       <c r="G16" t="n">
-        <v>0.01228091424798597</v>
+        <v>0.02799086804703515</v>
       </c>
       <c r="H16" t="n">
-        <v>0.005740165300891327</v>
+        <v>0.01019561362178679</v>
       </c>
       <c r="I16" t="n">
-        <v>0.00127092011451861</v>
+        <v>0.02099583857340922</v>
       </c>
       <c r="J16" t="n">
-        <v>0.04617706877145549</v>
+        <v>0.01790488106541976</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01569749939647684</v>
+        <v>0.007802602780508108</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0231548776538026</v>
+        <v>0.1022554721700806</v>
       </c>
       <c r="M16" t="n">
-        <v>0.02685084406719183</v>
+        <v>0.07033736450593542</v>
       </c>
       <c r="N16" t="n">
-        <v>0.01777589678062365</v>
+        <v>0.006254821165560967</v>
       </c>
       <c r="O16" t="n">
-        <v>0.05025825739729511</v>
+        <v>0.06637102294745602</v>
       </c>
       <c r="P16" t="n">
-        <v>0.01610458498943237</v>
+        <v>0.001833533634358156</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.09518751740690336</v>
+        <v>0.05335603446545024</v>
       </c>
       <c r="R16" t="n">
-        <v>0.08817300718880838</v>
+        <v>0.08458069621495699</v>
       </c>
       <c r="S16" t="n">
-        <v>0.06557200813112532</v>
+        <v>0.08237909100623232</v>
       </c>
       <c r="T16" t="n">
-        <v>0.01966689636712705</v>
+        <v>0.003010120123921585</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0929374848313996</v>
+        <v>0.05767438211363748</v>
       </c>
       <c r="V16" t="n">
-        <v>0.04910316313338513</v>
+        <v>0.004474810120564214</v>
       </c>
       <c r="W16" t="n">
-        <v>0.05607726567250016</v>
+        <v>0.02400418777646629</v>
       </c>
       <c r="X16" t="n">
-        <v>0.08593896027867519</v>
+        <v>0.08404767079120218</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.0541428968381509</v>
+        <v>0.05551338256547154</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.08355336748579492</v>
+        <v>0.09433800901888362</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.03244467054119126</v>
+        <v>0.03921752960996733</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.03155552954313363</v>
+        <v>0.01052834542032264</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.05081543578353018</v>
+        <v>0.02399024349947318</v>
       </c>
     </row>
     <row r="17">
@@ -2020,79 +2020,79 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.1689912927394101</v>
+        <v>0.1549357418645558</v>
       </c>
       <c r="F17" t="n">
-        <v>0.006426699303050248</v>
+        <v>0.03105908711852784</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01485740608363437</v>
+        <v>0.03235316768822472</v>
       </c>
       <c r="H17" t="n">
-        <v>0.04224631759929802</v>
+        <v>0.01606183290446243</v>
       </c>
       <c r="I17" t="n">
-        <v>0.08231181249311786</v>
+        <v>0.01733378339579498</v>
       </c>
       <c r="J17" t="n">
-        <v>0.06261995720837009</v>
+        <v>0.03536504592067991</v>
       </c>
       <c r="K17" t="n">
-        <v>0.09224992062809115</v>
+        <v>0.1001991660729881</v>
       </c>
       <c r="L17" t="n">
-        <v>0.08181718689476573</v>
+        <v>0.04242266613437791</v>
       </c>
       <c r="M17" t="n">
-        <v>0.05754625072529438</v>
+        <v>0.07256899615645548</v>
       </c>
       <c r="N17" t="n">
-        <v>0.02410184739300559</v>
+        <v>0.006732514365300777</v>
       </c>
       <c r="O17" t="n">
-        <v>0.05098603270047432</v>
+        <v>0.08651740337058091</v>
       </c>
       <c r="P17" t="n">
-        <v>0.08045098982730511</v>
+        <v>0.03644698658685697</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.006791637422716689</v>
+        <v>0.02260564280552482</v>
       </c>
       <c r="R17" t="n">
-        <v>0.03097873957569078</v>
+        <v>0.02597876025153823</v>
       </c>
       <c r="S17" t="n">
-        <v>0.04124146494356104</v>
+        <v>0.08529742481242351</v>
       </c>
       <c r="T17" t="n">
-        <v>0.08019287160563332</v>
+        <v>0.014266896107951</v>
       </c>
       <c r="U17" t="n">
-        <v>0.08792562075971831</v>
+        <v>0.0999720423364687</v>
       </c>
       <c r="V17" t="n">
-        <v>0.06299126869326857</v>
+        <v>0.03093939386249173</v>
       </c>
       <c r="W17" t="n">
-        <v>0.01075852220086307</v>
+        <v>0.1034116525715996</v>
       </c>
       <c r="X17" t="n">
-        <v>0.006868492548095795</v>
+        <v>0.03354280140250189</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.02774848677417417</v>
+        <v>0.01998988144125972</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.03963980615275738</v>
+        <v>0.002784042488832926</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.004405930655870554</v>
+        <v>0.08147139777476597</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.004842737811243652</v>
+        <v>0.002679414430391618</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.06395662319056102</v>
+        <v>0.06191905455263068</v>
       </c>
     </row>
     <row r="18">
@@ -2115,79 +2115,79 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.1232289042587866</v>
+        <v>0.1226790904901324</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04969436947104229</v>
+        <v>0.03705337948185932</v>
       </c>
       <c r="G18" t="n">
-        <v>0.07801997734627986</v>
+        <v>0.04432371640211426</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01785901774095223</v>
+        <v>0.0009590151646099233</v>
       </c>
       <c r="I18" t="n">
-        <v>0.002657732553461386</v>
+        <v>0.0006196468674300404</v>
       </c>
       <c r="J18" t="n">
-        <v>0.04957674324572863</v>
+        <v>0.07138093865813881</v>
       </c>
       <c r="K18" t="n">
-        <v>0.03423020752502317</v>
+        <v>0.005118498355416679</v>
       </c>
       <c r="L18" t="n">
-        <v>0.01730307194247114</v>
+        <v>0.04472151976689751</v>
       </c>
       <c r="M18" t="n">
-        <v>0.06241927198473228</v>
+        <v>0.02524416849594606</v>
       </c>
       <c r="N18" t="n">
-        <v>0.05467350230292373</v>
+        <v>0.04785313505795285</v>
       </c>
       <c r="O18" t="n">
-        <v>0.02562358488623577</v>
+        <v>0.05218920300060639</v>
       </c>
       <c r="P18" t="n">
-        <v>0.07568722979286592</v>
+        <v>0.03277986070893062</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.01499713832884994</v>
+        <v>0.01350031390283719</v>
       </c>
       <c r="R18" t="n">
-        <v>0.07630179835264661</v>
+        <v>0.08574720022316527</v>
       </c>
       <c r="S18" t="n">
-        <v>0.08102788501415756</v>
+        <v>0.08957784706367077</v>
       </c>
       <c r="T18" t="n">
-        <v>0.04575388582175986</v>
+        <v>0.0673551370345789</v>
       </c>
       <c r="U18" t="n">
-        <v>0.0239996520795395</v>
+        <v>0.02248042025024935</v>
       </c>
       <c r="V18" t="n">
-        <v>0.03057596419084369</v>
+        <v>0.04228591432770567</v>
       </c>
       <c r="W18" t="n">
-        <v>0.01217562627763302</v>
+        <v>0.008584965211241549</v>
       </c>
       <c r="X18" t="n">
-        <v>0.0203335367791166</v>
+        <v>0.03361374554827695</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.05269015972029917</v>
+        <v>0.06818961560099177</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.06599767071968324</v>
+        <v>0.09085615137549938</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.07398316779933801</v>
+        <v>0.07884255529303566</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.03441880612441624</v>
+        <v>0.03672305220884517</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.1242733592503509</v>
+        <v>0.09822504139550675</v>
       </c>
     </row>
     <row r="19">
@@ -2210,79 +2210,79 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.134725015207052</v>
+        <v>0.1378762370218201</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00640375717697822</v>
+        <v>0.009541460874259815</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03819530010542867</v>
+        <v>0.09968042671561043</v>
       </c>
       <c r="H19" t="n">
-        <v>0.03930059225149164</v>
+        <v>0.02525194194912138</v>
       </c>
       <c r="I19" t="n">
-        <v>0.05323074668668849</v>
+        <v>0.06355881647197902</v>
       </c>
       <c r="J19" t="n">
-        <v>0.01526006580880533</v>
+        <v>0.02787866840528661</v>
       </c>
       <c r="K19" t="n">
-        <v>0.04762373659997143</v>
+        <v>0.08533874058405029</v>
       </c>
       <c r="L19" t="n">
-        <v>0.05777228395273311</v>
+        <v>0.03767844016443258</v>
       </c>
       <c r="M19" t="n">
-        <v>0.007436096370984845</v>
+        <v>0.08909400094243429</v>
       </c>
       <c r="N19" t="n">
-        <v>0.01771573684513181</v>
+        <v>0.01313422614059347</v>
       </c>
       <c r="O19" t="n">
-        <v>0.01099429997284701</v>
+        <v>0.01296050000060712</v>
       </c>
       <c r="P19" t="n">
-        <v>0.1010453721115848</v>
+        <v>0.08498438445378853</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.01118807372352941</v>
+        <v>0.0358037157179589</v>
       </c>
       <c r="R19" t="n">
-        <v>0.08911897249194572</v>
+        <v>0.09964519987641689</v>
       </c>
       <c r="S19" t="n">
-        <v>0.08091529871753331</v>
+        <v>0.06008983477462605</v>
       </c>
       <c r="T19" t="n">
-        <v>0.09013845929425389</v>
+        <v>0.02830647650302832</v>
       </c>
       <c r="U19" t="n">
-        <v>0.03011757808331738</v>
+        <v>0.03674711952381197</v>
       </c>
       <c r="V19" t="n">
-        <v>0.07103527900834637</v>
+        <v>0.04851424698272464</v>
       </c>
       <c r="W19" t="n">
-        <v>0.04788350218479239</v>
+        <v>0.04926125063248361</v>
       </c>
       <c r="X19" t="n">
-        <v>0.05605903251051089</v>
+        <v>0.02313600291515734</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.002317458597928879</v>
+        <v>0.007259496434568161</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.03547731459303502</v>
+        <v>0.0447771527165606</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.001801849427441228</v>
+        <v>0.005982276583890866</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.08896919348472027</v>
+        <v>0.01137562063660904</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.1586922570810581</v>
+        <v>0.1793929330675016</v>
       </c>
     </row>
     <row r="20">
@@ -2305,79 +2305,79 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.1585097180636691</v>
+        <v>0.1583584266874534</v>
       </c>
       <c r="F20" t="n">
-        <v>0.04337152386120936</v>
+        <v>0.02673191704910808</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0218366999394791</v>
+        <v>0.07777821156522315</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0007894939430127765</v>
+        <v>0.03894771256291413</v>
       </c>
       <c r="I20" t="n">
-        <v>0.03688009727117289</v>
+        <v>0.01352769562242877</v>
       </c>
       <c r="J20" t="n">
-        <v>0.008282301845974598</v>
+        <v>0.01394801068724293</v>
       </c>
       <c r="K20" t="n">
-        <v>0.01117380233144636</v>
+        <v>0.04761487155823537</v>
       </c>
       <c r="L20" t="n">
-        <v>0.00508518789515814</v>
+        <v>0.02586660393888307</v>
       </c>
       <c r="M20" t="n">
-        <v>0.09276205978147406</v>
+        <v>0.0334350939650432</v>
       </c>
       <c r="N20" t="n">
-        <v>0.04862242072886289</v>
+        <v>0.1007072966115801</v>
       </c>
       <c r="O20" t="n">
-        <v>0.08126695916911858</v>
+        <v>0.06581453327538264</v>
       </c>
       <c r="P20" t="n">
-        <v>0.02150616398921708</v>
+        <v>0.002967304689788749</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.08160624378177861</v>
+        <v>0.04893731025653946</v>
       </c>
       <c r="R20" t="n">
-        <v>0.06438377539249455</v>
+        <v>0.007675114740241904</v>
       </c>
       <c r="S20" t="n">
-        <v>0.02872160060172683</v>
+        <v>0.06635925568045023</v>
       </c>
       <c r="T20" t="n">
-        <v>0.09232561502937869</v>
+        <v>0.005506441234133532</v>
       </c>
       <c r="U20" t="n">
-        <v>0.09553803330319073</v>
+        <v>0.07331396224181949</v>
       </c>
       <c r="V20" t="n">
-        <v>0.002501651048864019</v>
+        <v>0.00386037984887343</v>
       </c>
       <c r="W20" t="n">
-        <v>0.06880465809381296</v>
+        <v>0.02743920631514558</v>
       </c>
       <c r="X20" t="n">
-        <v>0.07915447613179724</v>
+        <v>0.08103424886035603</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.01173112515927369</v>
+        <v>0.02958716696670355</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.025415275138515</v>
+        <v>0.1017611714151567</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.05957664506826893</v>
+        <v>0.07577623685349283</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.018664190494773</v>
+        <v>0.03141025406125714</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.08675824368842779</v>
+        <v>0.07218269549107842</v>
       </c>
     </row>
     <row r="21">
@@ -2400,79 +2400,79 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.1657832649075941</v>
+        <v>0.1674007593705253</v>
       </c>
       <c r="F21" t="n">
-        <v>0.04690119429183961</v>
+        <v>0.08215583490698122</v>
       </c>
       <c r="G21" t="n">
-        <v>0.02343894444799177</v>
+        <v>0.08506602164873209</v>
       </c>
       <c r="H21" t="n">
-        <v>0.03613277174881906</v>
+        <v>0.02865450756884358</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001111512434370081</v>
+        <v>0.02517796904582398</v>
       </c>
       <c r="J21" t="n">
-        <v>0.08444394251262144</v>
+        <v>0.02256841437956006</v>
       </c>
       <c r="K21" t="n">
-        <v>0.05236562631678067</v>
+        <v>0.02987274365888383</v>
       </c>
       <c r="L21" t="n">
-        <v>0.02829063606874352</v>
+        <v>0.01478191317679654</v>
       </c>
       <c r="M21" t="n">
-        <v>0.00399028425455043</v>
+        <v>0.006246697302667513</v>
       </c>
       <c r="N21" t="n">
-        <v>0.02729418863517754</v>
+        <v>0.02556448973233114</v>
       </c>
       <c r="O21" t="n">
-        <v>0.05899421848720411</v>
+        <v>0.01376081290170483</v>
       </c>
       <c r="P21" t="n">
-        <v>0.008189285436071708</v>
+        <v>0.08106416932726221</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.01108214914415886</v>
+        <v>0.01739254118661382</v>
       </c>
       <c r="R21" t="n">
-        <v>0.08577192928749407</v>
+        <v>0.104678836958107</v>
       </c>
       <c r="S21" t="n">
-        <v>0.08406792389722799</v>
+        <v>0.09823469136918218</v>
       </c>
       <c r="T21" t="n">
-        <v>0.09092929509094785</v>
+        <v>0.06391571291234342</v>
       </c>
       <c r="U21" t="n">
-        <v>0.008156891552790847</v>
+        <v>0.0009623932730397177</v>
       </c>
       <c r="V21" t="n">
-        <v>0.1086594994482088</v>
+        <v>0.07467461298144328</v>
       </c>
       <c r="W21" t="n">
-        <v>0.07403426929481378</v>
+        <v>0.07167061628783344</v>
       </c>
       <c r="X21" t="n">
-        <v>0.0992495318797218</v>
+        <v>0.02093412914203182</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.01885837590508587</v>
+        <v>0.005415107524057452</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.026182001182371</v>
+        <v>0.04663544525802612</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.01080249713520576</v>
+        <v>0.05170999252023596</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.01105303154780331</v>
+        <v>0.02886234693749876</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.1117811153775061</v>
+        <v>0.1293680085271951</v>
       </c>
     </row>
     <row r="22">
@@ -2495,79 +2495,79 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.1737727034564796</v>
+        <v>0.1721744607712337</v>
       </c>
       <c r="F22" t="n">
-        <v>0.02682077884106496</v>
+        <v>0.09010086802458606</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0257137125045279</v>
+        <v>0.06766672268500763</v>
       </c>
       <c r="H22" t="n">
-        <v>0.002252425907173296</v>
+        <v>0.01138027397307495</v>
       </c>
       <c r="I22" t="n">
-        <v>0.004245620238436627</v>
+        <v>0.002988944126563287</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0280282239345745</v>
+        <v>0.002066754766432286</v>
       </c>
       <c r="K22" t="n">
-        <v>0.008473873959894232</v>
+        <v>0.01168783611161504</v>
       </c>
       <c r="L22" t="n">
-        <v>0.006037306464208498</v>
+        <v>0.03500728308261804</v>
       </c>
       <c r="M22" t="n">
-        <v>0.10191248673101</v>
+        <v>0.02497006900643083</v>
       </c>
       <c r="N22" t="n">
-        <v>0.003070238185357189</v>
+        <v>0.0001534646797371791</v>
       </c>
       <c r="O22" t="n">
-        <v>0.05511445902248539</v>
+        <v>0.05889128085474317</v>
       </c>
       <c r="P22" t="n">
-        <v>0.107766283049718</v>
+        <v>0.0117682464469321</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.05149631774216017</v>
+        <v>0.008364789690349291</v>
       </c>
       <c r="R22" t="n">
-        <v>0.007135716045247788</v>
+        <v>0.08160940875839405</v>
       </c>
       <c r="S22" t="n">
-        <v>0.02811310568225945</v>
+        <v>0.08318329260872516</v>
       </c>
       <c r="T22" t="n">
-        <v>0.02108739882055686</v>
+        <v>0.07596098574035694</v>
       </c>
       <c r="U22" t="n">
-        <v>0.06424058232254523</v>
+        <v>0.08981979158144555</v>
       </c>
       <c r="V22" t="n">
-        <v>0.04407728636957334</v>
+        <v>0.03090714247840918</v>
       </c>
       <c r="W22" t="n">
-        <v>0.103546386931348</v>
+        <v>0.08912898224558609</v>
       </c>
       <c r="X22" t="n">
-        <v>0.08563161579238646</v>
+        <v>0.08077756304925697</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.01418091446282844</v>
+        <v>0.02301250785355127</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.1050270556262854</v>
+        <v>0.06815257842571493</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.08387603494307376</v>
+        <v>0.01804416420111095</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.02215217642328429</v>
+        <v>0.03435704960935884</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.06388462923278392</v>
+        <v>0.05740081810730206</v>
       </c>
     </row>
     <row r="23">
@@ -2590,79 +2590,79 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.1871432512489913</v>
+        <v>0.1830763722971971</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1216780731255762</v>
+        <v>0.0888634434825971</v>
       </c>
       <c r="G23" t="n">
-        <v>0.02200712149550984</v>
+        <v>0.06891479211825284</v>
       </c>
       <c r="H23" t="n">
-        <v>0.04973011290025913</v>
+        <v>0.04926525259159784</v>
       </c>
       <c r="I23" t="n">
-        <v>0.02449027827262401</v>
+        <v>0.006132683912986725</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02729163425854047</v>
+        <v>0.009379510234061016</v>
       </c>
       <c r="K23" t="n">
-        <v>0.01658632975768443</v>
+        <v>0.02445459685552706</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0320738599981937</v>
+        <v>0.004268852492698731</v>
       </c>
       <c r="M23" t="n">
-        <v>0.04378753962294139</v>
+        <v>0.01141256907900434</v>
       </c>
       <c r="N23" t="n">
-        <v>0.02030800340810116</v>
+        <v>0.004873974844650281</v>
       </c>
       <c r="O23" t="n">
-        <v>0.01646389970195227</v>
+        <v>0.1000533103160074</v>
       </c>
       <c r="P23" t="n">
-        <v>0.02421457164111103</v>
+        <v>0.06192621157026219</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.06532328323529338</v>
+        <v>0.03920270957939964</v>
       </c>
       <c r="R23" t="n">
-        <v>0.04422154133719809</v>
+        <v>0.05367208175503181</v>
       </c>
       <c r="S23" t="n">
-        <v>0.03790521825057252</v>
+        <v>0.02809138444815833</v>
       </c>
       <c r="T23" t="n">
-        <v>0.02166006831067425</v>
+        <v>0.03828118030935554</v>
       </c>
       <c r="U23" t="n">
-        <v>0.00247334523721706</v>
+        <v>0.05202047822956444</v>
       </c>
       <c r="V23" t="n">
-        <v>0.1183603550902313</v>
+        <v>0.07425156412735742</v>
       </c>
       <c r="W23" t="n">
-        <v>0.05583711445644398</v>
+        <v>0.04240710340233302</v>
       </c>
       <c r="X23" t="n">
-        <v>0.05932343227196023</v>
+        <v>0.01105888777315371</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.004145233451997833</v>
+        <v>0.03972997866003438</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.07241019951541867</v>
+        <v>0.08502318415652783</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.1072090872720285</v>
+        <v>0.05139985751102251</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.01249969738847068</v>
+        <v>0.05531639255041576</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.0908128572653044</v>
+        <v>0.1089210370160845</v>
       </c>
     </row>
     <row r="24">
@@ -2685,79 +2685,79 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.1281863401693004</v>
+        <v>0.1277014799970706</v>
       </c>
       <c r="F24" t="n">
-        <v>0.08225551847158967</v>
+        <v>0.0783109856192294</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01565473154093391</v>
+        <v>0.05028207347553566</v>
       </c>
       <c r="H24" t="n">
-        <v>0.07574726702894537</v>
+        <v>0.07861704286883743</v>
       </c>
       <c r="I24" t="n">
-        <v>0.07669167486783125</v>
+        <v>0.02332795633392564</v>
       </c>
       <c r="J24" t="n">
-        <v>0.03410826938084619</v>
+        <v>0.005871502656259328</v>
       </c>
       <c r="K24" t="n">
-        <v>0.02122646200724396</v>
+        <v>0.04023671252612817</v>
       </c>
       <c r="L24" t="n">
-        <v>0.01961576909761046</v>
+        <v>0.00116975561143299</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0344264392060507</v>
+        <v>0.07608102335748031</v>
       </c>
       <c r="N24" t="n">
-        <v>0.003966162836704276</v>
+        <v>0.009501073626954014</v>
       </c>
       <c r="O24" t="n">
-        <v>0.01599668927332371</v>
+        <v>0.02464689548650398</v>
       </c>
       <c r="P24" t="n">
-        <v>0.08562251386062521</v>
+        <v>0.07106932125198018</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.005467435867968998</v>
+        <v>0.06375310798166478</v>
       </c>
       <c r="R24" t="n">
-        <v>0.00716242002128459</v>
+        <v>0.07199835997261624</v>
       </c>
       <c r="S24" t="n">
-        <v>0.04963830544797695</v>
+        <v>0.06711839449194437</v>
       </c>
       <c r="T24" t="n">
-        <v>0.05164755911795871</v>
+        <v>0.03156254469536857</v>
       </c>
       <c r="U24" t="n">
-        <v>0.06656471541762141</v>
+        <v>0.05366418998788446</v>
       </c>
       <c r="V24" t="n">
-        <v>0.0225128230962696</v>
+        <v>0.000631701406465743</v>
       </c>
       <c r="W24" t="n">
-        <v>0.06659499019292488</v>
+        <v>0.05410446381378491</v>
       </c>
       <c r="X24" t="n">
-        <v>0.0556949728845727</v>
+        <v>0.06077175895232493</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.03563304965333661</v>
+        <v>0.01552250310276432</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.06758249880619251</v>
+        <v>0.08105210944039237</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.04918397324619568</v>
+        <v>0.03258702258670153</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.05700575867599268</v>
+        <v>0.00811950075382064</v>
       </c>
       <c r="AC24" t="n">
-        <v>-0.1843562424644761</v>
+        <v>-0.175824545623544</v>
       </c>
     </row>
     <row r="25">
@@ -2780,79 +2780,79 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.15544577922385</v>
+        <v>0.1456390606113367</v>
       </c>
       <c r="F25" t="n">
-        <v>0.01561290757238702</v>
+        <v>0.1024840663672714</v>
       </c>
       <c r="G25" t="n">
-        <v>0.06497474947755436</v>
+        <v>0.08970267367558714</v>
       </c>
       <c r="H25" t="n">
-        <v>0.008463196160791848</v>
+        <v>0.03548306065892174</v>
       </c>
       <c r="I25" t="n">
-        <v>0.009225781885820463</v>
+        <v>0.08767422293320412</v>
       </c>
       <c r="J25" t="n">
-        <v>0.005019946001374963</v>
+        <v>0.02170797844970495</v>
       </c>
       <c r="K25" t="n">
-        <v>0.09192469099675232</v>
+        <v>0.0699078836515066</v>
       </c>
       <c r="L25" t="n">
-        <v>0.00781765021971882</v>
+        <v>0.01755338636466415</v>
       </c>
       <c r="M25" t="n">
-        <v>0.09344284010575669</v>
+        <v>0.07524248374272736</v>
       </c>
       <c r="N25" t="n">
-        <v>0.07097652077006464</v>
+        <v>0.01880087285556015</v>
       </c>
       <c r="O25" t="n">
-        <v>0.04749519578477944</v>
+        <v>0.02045356937993329</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1033933386382993</v>
+        <v>0.006244473578330171</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.1079667859491355</v>
+        <v>0.0772898106942822</v>
       </c>
       <c r="R25" t="n">
-        <v>0.0264333480248924</v>
+        <v>0.01777753244643127</v>
       </c>
       <c r="S25" t="n">
-        <v>0.01914566094155697</v>
+        <v>0.03354073360959294</v>
       </c>
       <c r="T25" t="n">
-        <v>0.02317031463125511</v>
+        <v>0.01473464822298303</v>
       </c>
       <c r="U25" t="n">
-        <v>0.009647399816883022</v>
+        <v>0.005306383821723947</v>
       </c>
       <c r="V25" t="n">
-        <v>0.04798171455184951</v>
+        <v>0.02698945825471444</v>
       </c>
       <c r="W25" t="n">
-        <v>0.0001906225737505841</v>
+        <v>0.002753225537712956</v>
       </c>
       <c r="X25" t="n">
-        <v>0.003096237206682273</v>
+        <v>0.02013856403680324</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.1084393395366672</v>
+        <v>0.1099697234459682</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.09995314847854206</v>
+        <v>0.0744883692485659</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.007665954928465136</v>
+        <v>0.0120746229137944</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.02796265574702048</v>
+        <v>0.05968225611001626</v>
       </c>
       <c r="AC25" t="n">
-        <v>-0.2033242246441314</v>
+        <v>-0.1815538442567368</v>
       </c>
     </row>
     <row r="26">
@@ -2875,79 +2875,79 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.1083956938650607</v>
+        <v>0.1098966192196796</v>
       </c>
       <c r="F26" t="n">
-        <v>0.03600080255262297</v>
+        <v>0.08283684458681677</v>
       </c>
       <c r="G26" t="n">
-        <v>0.08972287663735107</v>
+        <v>0.03503637657394414</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0384361333785091</v>
+        <v>0.002861907705306288</v>
       </c>
       <c r="I26" t="n">
-        <v>0.03077037362363157</v>
+        <v>0.0378861478862787</v>
       </c>
       <c r="J26" t="n">
-        <v>0.06111665625730936</v>
+        <v>0.06396805219752713</v>
       </c>
       <c r="K26" t="n">
-        <v>0.02155603013516261</v>
+        <v>0.01159393517993281</v>
       </c>
       <c r="L26" t="n">
-        <v>0.04592358998880981</v>
+        <v>0.03173656320102246</v>
       </c>
       <c r="M26" t="n">
-        <v>0.08174783713669541</v>
+        <v>0.09974124435321341</v>
       </c>
       <c r="N26" t="n">
-        <v>0.005315323570075967</v>
+        <v>0.03301257470123031</v>
       </c>
       <c r="O26" t="n">
-        <v>0.02402584880070489</v>
+        <v>0.004330800210784886</v>
       </c>
       <c r="P26" t="n">
-        <v>0.08565882632042054</v>
+        <v>0.02762882747437901</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.04239550139960856</v>
+        <v>0.09897899143718736</v>
       </c>
       <c r="R26" t="n">
-        <v>0.007044516171789903</v>
+        <v>0.04250861260925769</v>
       </c>
       <c r="S26" t="n">
-        <v>0.01182549273216225</v>
+        <v>0.001133725396044405</v>
       </c>
       <c r="T26" t="n">
-        <v>0.04272325973118123</v>
+        <v>0.01977098662831433</v>
       </c>
       <c r="U26" t="n">
-        <v>0.05766260353165584</v>
+        <v>0.09484127325063547</v>
       </c>
       <c r="V26" t="n">
-        <v>0.03155123997999016</v>
+        <v>0.02033731727708643</v>
       </c>
       <c r="W26" t="n">
-        <v>0.08339359850286282</v>
+        <v>0.08672280784899854</v>
       </c>
       <c r="X26" t="n">
-        <v>0.09176979126164317</v>
+        <v>0.06988296441237389</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.03232683770837545</v>
+        <v>0.06473823902681301</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.02070775191206117</v>
+        <v>0.03294118242423007</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.01229289258208578</v>
+        <v>0.0288494752176213</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.0460322160852905</v>
+        <v>0.008661150401001504</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.1734012451094805</v>
+        <v>0.1789199580089839</v>
       </c>
     </row>
     <row r="27">
@@ -2970,79 +2970,79 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.1208478080364496</v>
+        <v>0.1181224077812383</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0973442428917141</v>
+        <v>0.09680440313310275</v>
       </c>
       <c r="G27" t="n">
-        <v>0.03994835456442144</v>
+        <v>0.01251573428260763</v>
       </c>
       <c r="H27" t="n">
-        <v>0.004367231917367131</v>
+        <v>0.06019033541922458</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0002961469858244063</v>
+        <v>0.004785766295726491</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0200221095256985</v>
+        <v>0.04868048235946981</v>
       </c>
       <c r="K27" t="n">
-        <v>0.04037060117840251</v>
+        <v>0.008252229874686877</v>
       </c>
       <c r="L27" t="n">
-        <v>0.02016061960725497</v>
+        <v>0.0289341046402574</v>
       </c>
       <c r="M27" t="n">
-        <v>0.08899594748888548</v>
+        <v>0.08112883670289335</v>
       </c>
       <c r="N27" t="n">
-        <v>0.0027899273393136</v>
+        <v>0.006384973087465031</v>
       </c>
       <c r="O27" t="n">
-        <v>0.05423610204832412</v>
+        <v>0.07171047299020361</v>
       </c>
       <c r="P27" t="n">
-        <v>0.01535480322181451</v>
+        <v>0.0005296956776903033</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.0777064252078042</v>
+        <v>0.07619018216941974</v>
       </c>
       <c r="R27" t="n">
-        <v>0.07101586692045816</v>
+        <v>0.02738096913642708</v>
       </c>
       <c r="S27" t="n">
-        <v>0.0107833864546037</v>
+        <v>0.002050978718666584</v>
       </c>
       <c r="T27" t="n">
-        <v>0.02717032666571757</v>
+        <v>0.06004852118993569</v>
       </c>
       <c r="U27" t="n">
-        <v>0.00136675951670251</v>
+        <v>0.02188948757920895</v>
       </c>
       <c r="V27" t="n">
-        <v>0.06189460899939703</v>
+        <v>0.002979303701765267</v>
       </c>
       <c r="W27" t="n">
-        <v>0.08358881439443097</v>
+        <v>0.004874351925424885</v>
       </c>
       <c r="X27" t="n">
-        <v>0.04957956188947565</v>
+        <v>0.06909914037909447</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.07245580849918663</v>
+        <v>0.106957194009099</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.0008254368555441346</v>
+        <v>0.08840329095435348</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.07844443026112881</v>
+        <v>0.04154293258304714</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.0812824875665298</v>
+        <v>0.07866661319022973</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.2189315911454672</v>
+        <v>0.2436410101955782</v>
       </c>
     </row>
     <row r="28">
@@ -3065,79 +3065,79 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.113018233020884</v>
+        <v>0.1128369247015725</v>
       </c>
       <c r="F28" t="n">
-        <v>0.01478205134492583</v>
+        <v>0.02426017723808054</v>
       </c>
       <c r="G28" t="n">
-        <v>0.04012944885773265</v>
+        <v>0.03825120300174639</v>
       </c>
       <c r="H28" t="n">
-        <v>0.02150111876677596</v>
+        <v>0.02673403120723409</v>
       </c>
       <c r="I28" t="n">
-        <v>0.04274190139483083</v>
+        <v>0.07169087007110557</v>
       </c>
       <c r="J28" t="n">
-        <v>0.06814460319579239</v>
+        <v>0.0566015298747887</v>
       </c>
       <c r="K28" t="n">
-        <v>0.02714206932434389</v>
+        <v>0.009437710126279751</v>
       </c>
       <c r="L28" t="n">
-        <v>0.04386545010233455</v>
+        <v>0.02269020788336277</v>
       </c>
       <c r="M28" t="n">
-        <v>0.09152081375606327</v>
+        <v>0.05167485837627247</v>
       </c>
       <c r="N28" t="n">
-        <v>0.0261849871130175</v>
+        <v>0.01127333622125807</v>
       </c>
       <c r="O28" t="n">
-        <v>0.03707946793244467</v>
+        <v>0.08263399842540199</v>
       </c>
       <c r="P28" t="n">
-        <v>0.07314503943787531</v>
+        <v>0.113190473380505</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.08374549653786596</v>
+        <v>0.09433167671797985</v>
       </c>
       <c r="R28" t="n">
-        <v>0.001244511926666499</v>
+        <v>0.02865983538396443</v>
       </c>
       <c r="S28" t="n">
-        <v>0.03217588946241854</v>
+        <v>0.05794684050507909</v>
       </c>
       <c r="T28" t="n">
-        <v>0.06249796935786976</v>
+        <v>0.05844608559787932</v>
       </c>
       <c r="U28" t="n">
-        <v>0.07559648407466839</v>
+        <v>0.1058338376157519</v>
       </c>
       <c r="V28" t="n">
-        <v>8.374415357930603e-05</v>
+        <v>0.02093050762467488</v>
       </c>
       <c r="W28" t="n">
-        <v>0.05494059296438525</v>
+        <v>0.03017595613887927</v>
       </c>
       <c r="X28" t="n">
-        <v>0.08412890399300418</v>
+        <v>0.0736924158801765</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.03488227282246584</v>
+        <v>0.01072654994292624</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.03965874208329202</v>
+        <v>0.004652079103332744</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.00641011717461555</v>
+        <v>0.001921935696138089</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.03839832422303168</v>
+        <v>0.004243883987182505</v>
       </c>
       <c r="AC28" t="n">
-        <v>-0.01756493767786431</v>
+        <v>-0.02621985065443563</v>
       </c>
     </row>
     <row r="29">
@@ -3160,79 +3160,79 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.1197469009782979</v>
+        <v>0.1289371981502553</v>
       </c>
       <c r="F29" t="n">
-        <v>0.04695672092155241</v>
+        <v>0.07650087793685358</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0489192334450963</v>
+        <v>0.07161003661584894</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01614512236006596</v>
+        <v>0.01608365677625261</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01473002510374686</v>
+        <v>0.005161828515796929</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0160114851196445</v>
+        <v>0.004211455119836419</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0052450848151216</v>
+        <v>0.004215788513201201</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01914412744567632</v>
+        <v>0.02106056358451616</v>
       </c>
       <c r="M29" t="n">
-        <v>0.06836605238134463</v>
+        <v>0.08136429850953805</v>
       </c>
       <c r="N29" t="n">
-        <v>0.04826444702830503</v>
+        <v>0.03202931207955671</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0857852047296596</v>
+        <v>0.06445687027765776</v>
       </c>
       <c r="P29" t="n">
-        <v>0.04479405980937311</v>
+        <v>0.04105517491674265</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.03955762007192945</v>
+        <v>0.03878908977995209</v>
       </c>
       <c r="R29" t="n">
-        <v>0.08887335531605831</v>
+        <v>0.01358327342465274</v>
       </c>
       <c r="S29" t="n">
-        <v>0.003418954417909736</v>
+        <v>0.05927902400464781</v>
       </c>
       <c r="T29" t="n">
-        <v>0.029822626542709</v>
+        <v>0.003520384470005488</v>
       </c>
       <c r="U29" t="n">
-        <v>0.05295230132062427</v>
+        <v>0.05099799432028621</v>
       </c>
       <c r="V29" t="n">
-        <v>0.01239535286912941</v>
+        <v>0.06088714825379659</v>
       </c>
       <c r="W29" t="n">
-        <v>0.09542884237708021</v>
+        <v>0.04478960504637512</v>
       </c>
       <c r="X29" t="n">
-        <v>0.03429845153354946</v>
+        <v>0.05565335443393343</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.09786951591546787</v>
+        <v>0.08426065500053312</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.03833337543144104</v>
+        <v>0.08226068162958011</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.0673885093287982</v>
+        <v>0.03314709591461926</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.02529953171571678</v>
+        <v>0.05508183087581693</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.05747421770935431</v>
+        <v>0.02731793180617974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>